<commit_message>
messages storing rework | add console logger
</commit_message>
<xml_diff>
--- a/StatisticTable.xlsx
+++ b/StatisticTable.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
   <si>
     <t>telegram ID</t>
   </si>
@@ -47,6 +47,27 @@
     <t>Должность</t>
   </si>
   <si>
+    <t>juliaarxi</t>
+  </si>
+  <si>
+    <t>Юля Архипова</t>
+  </si>
+  <si>
+    <t>Администратор</t>
+  </si>
+  <si>
+    <t>Юлия</t>
+  </si>
+  <si>
+    <t>julila.arxi@gmail.com</t>
+  </si>
+  <si>
+    <t>+79996194821</t>
+  </si>
+  <si>
+    <t>Не заполненно</t>
+  </si>
+  <si>
     <t>agfnkit</t>
   </si>
   <si>
@@ -56,40 +77,43 @@
     <t>Резидент</t>
   </si>
   <si>
-    <t>Никита</t>
-  </si>
-  <si>
-    <t>2636</t>
-  </si>
-  <si>
-    <t>777777</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>аав</t>
-  </si>
-  <si>
-    <t>K0T_ya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Катя </t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test@test.ru</t>
+  </si>
+  <si>
+    <t>+79999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Незарегестрирован</t>
+  </si>
+  <si>
+    <t>kuzlyaevnikita</t>
+  </si>
+  <si>
+    <t>Никита Кузляев</t>
+  </si>
+  <si>
+    <t>X1STY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1STY </t>
   </si>
   <si>
     <t>Агент поддержки</t>
   </si>
   <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>log@log.rs</t>
-  </si>
-  <si>
-    <t>12123123132</t>
-  </si>
-  <si>
-    <t>Не заполненно</t>
+    <t>Шмфт</t>
+  </si>
+  <si>
+    <t>asdsd@asdas.ru</t>
+  </si>
+  <si>
+    <t>89887886655</t>
   </si>
   <si>
     <t>iat39</t>
@@ -98,34 +122,13 @@
     <t>Иван Толканюк</t>
   </si>
   <si>
-    <t>Gg</t>
-  </si>
-  <si>
-    <t>Hg</t>
-  </si>
-  <si>
-    <t>Hh</t>
-  </si>
-  <si>
-    <t>X1STY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X1STY </t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>kuzlyaevnikita</t>
-  </si>
-  <si>
-    <t>Никита Кузляев</t>
-  </si>
-  <si>
-    <t>Незарегестрирован</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>d@df.ru</t>
+  </si>
+  <si>
+    <t>89999999999</t>
   </si>
   <si>
     <t>Номер заявки</t>
@@ -185,18 +188,6 @@
     <t>Планируемый объем инвестиций</t>
   </si>
   <si>
-    <t>В ожидании</t>
-  </si>
-  <si>
-    <t>14.11.2023, 13:44:57</t>
-  </si>
-  <si>
-    <t>Не закреплен</t>
-  </si>
-  <si>
-    <t>Не обработана</t>
-  </si>
-  <si>
     <t>Тип площади</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
   </si>
   <si>
     <t>Выбранный корпус</t>
-  </si>
-  <si>
-    <t>14.11.2023, 13:45:04</t>
   </si>
   <si>
     <t>Описание проблемы</t>
@@ -607,14 +595,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="6" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="9" width="16" customWidth="1"/>
   </cols>
@@ -650,7 +639,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>516116895</v>
+        <v>99028179</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -674,123 +663,152 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>875877003</v>
+        <v>516116895</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1974140479</v>
+        <v>5996444666</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>265531301</v>
+        <v>1174135298</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1174135298</v>
+        <v>265531301</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1974140479</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -818,34 +836,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -874,37 +892,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -930,28 +948,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +980,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -970,7 +988,7 @@
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
@@ -978,60 +996,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2">
-        <v>1974140479</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1031,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -1051,7 +1040,7 @@
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
@@ -1059,63 +1048,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2">
-        <v>1974140479</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1141,28 +1101,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1190,37 +1150,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>